<commit_message>
Changes made to start Poland Microsimulaiton Model
</commit_message>
<xml_diff>
--- a/Poland CIT Sample.xlsx
+++ b/Poland CIT Sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb305167\OneDrive - WBG\Other Missions\Poland\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb305167\Documents\python\Microsimulation\Microsimulation_Poland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548B4649-8F50-45DB-B45C-B272F7273F8A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E116E1F9-3D43-4BB5-8D8D-7CC552A07BBD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dane dla BŚ" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2949" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2951" uniqueCount="195">
   <si>
     <t>Szczególna forma prawna</t>
   </si>
@@ -618,9 +618,6 @@
     <t>06 Lublin Province</t>
   </si>
   <si>
-    <t>10 Łódź Province</t>
-  </si>
-  <si>
     <t>12 Lesser Poland Province</t>
   </si>
   <si>
@@ -636,9 +633,6 @@
     <t>24 Silesia Province</t>
   </si>
   <si>
-    <t>26 Świętokrzyskie Province</t>
-  </si>
-  <si>
     <t>30 Greater Poland Province</t>
   </si>
   <si>
@@ -646,6 +640,12 @@
   </si>
   <si>
     <t>28 Warmian-Masurian Province</t>
+  </si>
+  <si>
+    <t>26 Swietokrzyskie Province</t>
+  </si>
+  <si>
+    <t>10 Lodz</t>
   </si>
 </sst>
 </file>
@@ -831,9 +831,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -842,6 +839,9 @@
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1154,17 +1154,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
       <c r="L1" s="24"/>
@@ -34845,8 +34845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCEBCF2-7BCD-464C-9CC3-58FC2DD939B9}">
   <dimension ref="A1:AT454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="E301" workbookViewId="0">
+      <selection activeCell="F330" sqref="F330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -34887,143 +34887,143 @@
     <col min="47" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="30" customFormat="1" ht="66" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:46" s="29" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="Q1" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="S1" s="29" t="s">
+      <c r="S1" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="T1" s="29" t="s">
+      <c r="T1" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="U1" s="29" t="s">
+      <c r="U1" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="V1" s="29" t="s">
+      <c r="V1" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="W1" s="29" t="s">
+      <c r="W1" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="X1" s="29" t="s">
+      <c r="X1" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="29" t="s">
+      <c r="Y1" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="Z1" s="29" t="s">
+      <c r="Z1" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="AA1" s="29" t="s">
+      <c r="AA1" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="29" t="s">
+      <c r="AB1" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="AC1" s="29" t="s">
+      <c r="AC1" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="AD1" s="29" t="s">
+      <c r="AD1" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="AE1" s="29" t="s">
+      <c r="AE1" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="AF1" s="29" t="s">
+      <c r="AF1" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="AG1" s="29" t="s">
+      <c r="AG1" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="AH1" s="29" t="s">
+      <c r="AH1" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="AI1" s="29" t="s">
+      <c r="AI1" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="AJ1" s="29" t="s">
+      <c r="AJ1" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="AK1" s="29" t="s">
+      <c r="AK1" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="AL1" s="29" t="s">
+      <c r="AL1" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="AM1" s="29" t="s">
+      <c r="AM1" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="AN1" s="29" t="s">
+      <c r="AN1" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="AO1" s="29" t="s">
+      <c r="AO1" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="AP1" s="29" t="s">
+      <c r="AP1" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="AQ1" s="29" t="s">
+      <c r="AQ1" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="AR1" s="29" t="s">
+      <c r="AR1" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="AS1" s="29" t="s">
+      <c r="AS1" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="AT1" s="29" t="s">
+      <c r="AT1" s="28" t="s">
         <v>142</v>
       </c>
     </row>
@@ -35385,7 +35385,7 @@
         <v>39</v>
       </c>
       <c r="G5" s="26" t="str">
-        <f>VLOOKUP(F5,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F5,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H5" s="16">
@@ -35472,8 +35472,8 @@
         <v>63</v>
       </c>
       <c r="G6" s="26" t="str">
-        <f>VLOOKUP(F6,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>26 Świętokrzyskie Province</v>
+        <f>VLOOKUP(F6,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>26 Swietokrzyskie Province</v>
       </c>
       <c r="H6" s="16">
         <v>106987524.3</v>
@@ -35559,7 +35559,7 @@
         <v>39</v>
       </c>
       <c r="G7" s="26" t="str">
-        <f>VLOOKUP(F7,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F7,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H7" s="16">
@@ -35650,7 +35650,7 @@
         <v>53</v>
       </c>
       <c r="G8" s="26" t="str">
-        <f>VLOOKUP(F8,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F8,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H8" s="16">
@@ -35741,7 +35741,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="26" t="str">
-        <f>VLOOKUP(F9,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F9,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H9" s="16">
@@ -35832,7 +35832,7 @@
         <v>47</v>
       </c>
       <c r="G10" s="26" t="str">
-        <f>VLOOKUP(F10,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F10,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H10" s="16">
@@ -35923,7 +35923,7 @@
         <v>39</v>
       </c>
       <c r="G11" s="26" t="str">
-        <f>VLOOKUP(F11,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F11,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H11" s="16">
@@ -36010,8 +36010,8 @@
         <v>57</v>
       </c>
       <c r="G12" s="26" t="str">
-        <f>VLOOKUP(F12,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F12,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H12" s="16">
         <v>27251986.559999999</v>
@@ -36097,8 +36097,8 @@
         <v>63</v>
       </c>
       <c r="G13" s="26" t="str">
-        <f>VLOOKUP(F13,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>26 Świętokrzyskie Province</v>
+        <f>VLOOKUP(F13,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>26 Swietokrzyskie Province</v>
       </c>
       <c r="H13" s="16">
         <v>19983182.98</v>
@@ -36184,7 +36184,7 @@
         <v>39</v>
       </c>
       <c r="G14" s="26" t="str">
-        <f>VLOOKUP(F14,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F14,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H14" s="16">
@@ -36271,7 +36271,7 @@
         <v>39</v>
       </c>
       <c r="G15" s="26" t="str">
-        <f>VLOOKUP(F15,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F15,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H15" s="16">
@@ -36358,7 +36358,7 @@
         <v>42</v>
       </c>
       <c r="G16" s="26" t="str">
-        <f>VLOOKUP(F16,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F16,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H16" s="16">
@@ -36445,8 +36445,8 @@
         <v>57</v>
       </c>
       <c r="G17" s="26" t="str">
-        <f>VLOOKUP(F17,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F17,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H17" s="16">
         <v>11712683.959999999</v>
@@ -36536,7 +36536,7 @@
         <v>47</v>
       </c>
       <c r="G18" s="26" t="str">
-        <f>VLOOKUP(F18,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F18,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H18" s="16">
@@ -36627,7 +36627,7 @@
         <v>39</v>
       </c>
       <c r="G19" s="26" t="str">
-        <f>VLOOKUP(F19,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F19,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H19" s="16">
@@ -36718,7 +36718,7 @@
         <v>53</v>
       </c>
       <c r="G20" s="26" t="str">
-        <f>VLOOKUP(F20,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F20,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H20" s="16">
@@ -36809,7 +36809,7 @@
         <v>39</v>
       </c>
       <c r="G21" s="26" t="str">
-        <f>VLOOKUP(F21,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F21,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H21" s="16">
@@ -36900,7 +36900,7 @@
         <v>39</v>
       </c>
       <c r="G22" s="26" t="str">
-        <f>VLOOKUP(F22,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F22,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H22" s="16">
@@ -36991,7 +36991,7 @@
         <v>51</v>
       </c>
       <c r="G23" s="26" t="str">
-        <f>VLOOKUP(F23,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F23,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H23" s="16">
@@ -37080,7 +37080,7 @@
         <v>53</v>
       </c>
       <c r="G24" s="26" t="str">
-        <f>VLOOKUP(F24,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F24,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H24" s="16">
@@ -37167,7 +37167,7 @@
         <v>42</v>
       </c>
       <c r="G25" s="26" t="str">
-        <f>VLOOKUP(F25,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F25,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H25" s="16">
@@ -37254,7 +37254,7 @@
         <v>42</v>
       </c>
       <c r="G26" s="26" t="str">
-        <f>VLOOKUP(F26,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F26,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H26" s="16">
@@ -37345,7 +37345,7 @@
         <v>39</v>
       </c>
       <c r="G27" s="26" t="str">
-        <f>VLOOKUP(F27,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F27,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H27" s="14">
@@ -37428,8 +37428,8 @@
         <v>63</v>
       </c>
       <c r="G28" s="26" t="str">
-        <f>VLOOKUP(F28,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>26 Świętokrzyskie Province</v>
+        <f>VLOOKUP(F28,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>26 Swietokrzyskie Province</v>
       </c>
       <c r="H28" s="14">
         <v>8694420.0800000001</v>
@@ -37511,8 +37511,8 @@
         <v>63</v>
       </c>
       <c r="G29" s="26" t="str">
-        <f>VLOOKUP(F29,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>26 Świętokrzyskie Province</v>
+        <f>VLOOKUP(F29,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>26 Swietokrzyskie Province</v>
       </c>
       <c r="H29" s="14">
         <v>8694359.1699999999</v>
@@ -37594,7 +37594,7 @@
         <v>42</v>
       </c>
       <c r="G30" s="26" t="str">
-        <f>VLOOKUP(F30,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F30,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H30" s="14">
@@ -37693,8 +37693,8 @@
         <v>57</v>
       </c>
       <c r="G31" s="26" t="str">
-        <f>VLOOKUP(F31,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F31,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H31" s="14">
         <v>8693160.0299999993</v>
@@ -37780,7 +37780,7 @@
         <v>47</v>
       </c>
       <c r="G32" s="26" t="str">
-        <f>VLOOKUP(F32,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F32,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H32" s="14">
@@ -37867,7 +37867,7 @@
         <v>39</v>
       </c>
       <c r="G33" s="26" t="str">
-        <f>VLOOKUP(F33,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F33,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H33" s="14">
@@ -37954,7 +37954,7 @@
         <v>53</v>
       </c>
       <c r="G34" s="26" t="str">
-        <f>VLOOKUP(F34,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F34,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H34" s="14">
@@ -38037,7 +38037,7 @@
         <v>39</v>
       </c>
       <c r="G35" s="26" t="str">
-        <f>VLOOKUP(F35,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F35,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H35" s="14">
@@ -38124,7 +38124,7 @@
         <v>39</v>
       </c>
       <c r="G36" s="26" t="str">
-        <f>VLOOKUP(F36,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F36,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H36" s="14">
@@ -38203,7 +38203,7 @@
         <v>39</v>
       </c>
       <c r="G37" s="26" t="str">
-        <f>VLOOKUP(F37,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F37,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H37" s="14">
@@ -38290,7 +38290,7 @@
         <v>39</v>
       </c>
       <c r="G38" s="26" t="str">
-        <f>VLOOKUP(F38,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F38,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H38" s="14">
@@ -38381,7 +38381,7 @@
         <v>39</v>
       </c>
       <c r="G39" s="26" t="str">
-        <f>VLOOKUP(F39,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F39,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H39" s="14">
@@ -38468,7 +38468,7 @@
         <v>53</v>
       </c>
       <c r="G40" s="26" t="str">
-        <f>VLOOKUP(F40,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F40,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H40" s="14">
@@ -38555,7 +38555,7 @@
         <v>39</v>
       </c>
       <c r="G41" s="26" t="str">
-        <f>VLOOKUP(F41,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F41,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H41" s="14">
@@ -38642,7 +38642,7 @@
         <v>53</v>
       </c>
       <c r="G42" s="26" t="str">
-        <f>VLOOKUP(F42,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F42,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H42" s="14">
@@ -38729,7 +38729,7 @@
         <v>53</v>
       </c>
       <c r="G43" s="26" t="str">
-        <f>VLOOKUP(F43,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F43,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H43" s="14">
@@ -38820,7 +38820,7 @@
         <v>53</v>
       </c>
       <c r="G44" s="26" t="str">
-        <f>VLOOKUP(F44,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F44,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H44" s="14">
@@ -38911,7 +38911,7 @@
         <v>51</v>
       </c>
       <c r="G45" s="26" t="str">
-        <f>VLOOKUP(F45,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F45,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H45" s="14">
@@ -38998,7 +38998,7 @@
         <v>56</v>
       </c>
       <c r="G46" s="26" t="str">
-        <f>VLOOKUP(F46,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F46,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H46" s="14">
@@ -39085,7 +39085,7 @@
         <v>56</v>
       </c>
       <c r="G47" s="26" t="str">
-        <f>VLOOKUP(F47,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F47,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H47" s="14">
@@ -39180,7 +39180,7 @@
         <v>53</v>
       </c>
       <c r="G48" s="26" t="str">
-        <f>VLOOKUP(F48,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F48,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H48" s="14">
@@ -39267,7 +39267,7 @@
         <v>42</v>
       </c>
       <c r="G49" s="26" t="str">
-        <f>VLOOKUP(F49,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F49,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H49" s="14">
@@ -39354,7 +39354,7 @@
         <v>47</v>
       </c>
       <c r="G50" s="26" t="str">
-        <f>VLOOKUP(F50,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F50,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H50" s="14">
@@ -39441,7 +39441,7 @@
         <v>51</v>
       </c>
       <c r="G51" s="26" t="str">
-        <f>VLOOKUP(F51,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F51,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H51" s="14">
@@ -39534,7 +39534,7 @@
         <v>51</v>
       </c>
       <c r="G52" s="26" t="str">
-        <f>VLOOKUP(F52,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F52,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H52" s="14">
@@ -39621,7 +39621,7 @@
         <v>39</v>
       </c>
       <c r="G53" s="26" t="str">
-        <f>VLOOKUP(F53,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F53,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H53" s="14">
@@ -39708,7 +39708,7 @@
         <v>56</v>
       </c>
       <c r="G54" s="26" t="str">
-        <f>VLOOKUP(F54,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F54,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H54" s="14">
@@ -39787,7 +39787,7 @@
         <v>51</v>
       </c>
       <c r="G55" s="26" t="str">
-        <f>VLOOKUP(F55,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F55,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H55" s="14">
@@ -39874,7 +39874,7 @@
         <v>53</v>
       </c>
       <c r="G56" s="26" t="str">
-        <f>VLOOKUP(F56,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F56,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H56" s="14">
@@ -39965,7 +39965,7 @@
         <v>53</v>
       </c>
       <c r="G57" s="26" t="str">
-        <f>VLOOKUP(F57,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F57,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H57" s="14">
@@ -40044,7 +40044,7 @@
         <v>39</v>
       </c>
       <c r="G58" s="26" t="str">
-        <f>VLOOKUP(F58,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F58,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H58" s="14">
@@ -40135,7 +40135,7 @@
         <v>39</v>
       </c>
       <c r="G59" s="26" t="str">
-        <f>VLOOKUP(F59,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F59,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H59" s="14">
@@ -40222,7 +40222,7 @@
         <v>47</v>
       </c>
       <c r="G60" s="26" t="str">
-        <f>VLOOKUP(F60,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F60,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H60" s="14">
@@ -40301,8 +40301,8 @@
         <v>57</v>
       </c>
       <c r="G61" s="26" t="str">
-        <f>VLOOKUP(F61,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F61,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H61" s="14">
         <v>8671001.5500000007</v>
@@ -40392,7 +40392,7 @@
         <v>39</v>
       </c>
       <c r="G62" s="26" t="str">
-        <f>VLOOKUP(F62,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F62,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H62" s="14">
@@ -40471,7 +40471,7 @@
         <v>42</v>
       </c>
       <c r="G63" s="26" t="str">
-        <f>VLOOKUP(F63,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F63,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H63" s="14">
@@ -40562,7 +40562,7 @@
         <v>39</v>
       </c>
       <c r="G64" s="26" t="str">
-        <f>VLOOKUP(F64,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F64,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H64" s="14">
@@ -40641,7 +40641,7 @@
         <v>39</v>
       </c>
       <c r="G65" s="26" t="str">
-        <f>VLOOKUP(F65,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F65,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H65" s="14">
@@ -40728,7 +40728,7 @@
         <v>53</v>
       </c>
       <c r="G66" s="26" t="str">
-        <f>VLOOKUP(F66,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F66,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H66" s="14">
@@ -40819,7 +40819,7 @@
         <v>39</v>
       </c>
       <c r="G67" s="26" t="str">
-        <f>VLOOKUP(F67,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F67,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H67" s="14">
@@ -40906,7 +40906,7 @@
         <v>47</v>
       </c>
       <c r="G68" s="26" t="str">
-        <f>VLOOKUP(F68,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F68,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H68" s="14">
@@ -40997,7 +40997,7 @@
         <v>39</v>
       </c>
       <c r="G69" s="26" t="str">
-        <f>VLOOKUP(F69,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F69,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H69" s="14">
@@ -41084,7 +41084,7 @@
         <v>42</v>
       </c>
       <c r="G70" s="26" t="str">
-        <f>VLOOKUP(F70,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F70,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H70" s="14">
@@ -41163,7 +41163,7 @@
         <v>51</v>
       </c>
       <c r="G71" s="26" t="str">
-        <f>VLOOKUP(F71,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F71,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H71" s="14">
@@ -41250,7 +41250,7 @@
         <v>39</v>
       </c>
       <c r="G72" s="26" t="str">
-        <f>VLOOKUP(F72,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F72,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H72" s="14">
@@ -41337,7 +41337,7 @@
         <v>56</v>
       </c>
       <c r="G73" s="26" t="str">
-        <f>VLOOKUP(F73,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F73,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H73" s="14">
@@ -41424,7 +41424,7 @@
         <v>39</v>
       </c>
       <c r="G74" s="26" t="str">
-        <f>VLOOKUP(F74,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F74,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H74" s="14">
@@ -41515,8 +41515,8 @@
         <v>57</v>
       </c>
       <c r="G75" s="26" t="str">
-        <f>VLOOKUP(F75,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F75,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H75" s="14">
         <v>8665838.3000000007</v>
@@ -41602,7 +41602,7 @@
         <v>51</v>
       </c>
       <c r="G76" s="26" t="str">
-        <f>VLOOKUP(F76,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F76,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H76" s="14">
@@ -41693,7 +41693,7 @@
         <v>42</v>
       </c>
       <c r="G77" s="26" t="str">
-        <f>VLOOKUP(F77,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F77,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H77" s="14">
@@ -41772,7 +41772,7 @@
         <v>47</v>
       </c>
       <c r="G78" s="26" t="str">
-        <f>VLOOKUP(F78,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F78,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H78" s="14">
@@ -41859,7 +41859,7 @@
         <v>39</v>
       </c>
       <c r="G79" s="26" t="str">
-        <f>VLOOKUP(F79,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F79,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H79" s="14">
@@ -41946,7 +41946,7 @@
         <v>51</v>
       </c>
       <c r="G80" s="26" t="str">
-        <f>VLOOKUP(F80,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F80,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H80" s="14">
@@ -42033,7 +42033,7 @@
         <v>42</v>
       </c>
       <c r="G81" s="26" t="str">
-        <f>VLOOKUP(F81,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F81,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H81" s="14">
@@ -42124,7 +42124,7 @@
         <v>53</v>
       </c>
       <c r="G82" s="26" t="str">
-        <f>VLOOKUP(F82,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F82,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H82" s="14">
@@ -42211,7 +42211,7 @@
         <v>39</v>
       </c>
       <c r="G83" s="26" t="str">
-        <f>VLOOKUP(F83,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F83,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H83" s="14">
@@ -42296,7 +42296,7 @@
         <v>53</v>
       </c>
       <c r="G84" s="26" t="str">
-        <f>VLOOKUP(F84,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F84,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H84" s="14">
@@ -42387,7 +42387,7 @@
         <v>39</v>
       </c>
       <c r="G85" s="26" t="str">
-        <f>VLOOKUP(F85,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F85,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H85" s="14">
@@ -42466,7 +42466,7 @@
         <v>39</v>
       </c>
       <c r="G86" s="26" t="str">
-        <f>VLOOKUP(F86,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F86,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H86" s="14">
@@ -42549,7 +42549,7 @@
         <v>51</v>
       </c>
       <c r="G87" s="26" t="str">
-        <f>VLOOKUP(F87,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F87,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H87" s="14">
@@ -42636,7 +42636,7 @@
         <v>39</v>
       </c>
       <c r="G88" s="26" t="str">
-        <f>VLOOKUP(F88,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F88,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H88" s="14">
@@ -42715,7 +42715,7 @@
         <v>39</v>
       </c>
       <c r="G89" s="26" t="str">
-        <f>VLOOKUP(F89,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F89,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H89" s="14">
@@ -42802,7 +42802,7 @@
         <v>39</v>
       </c>
       <c r="G90" s="26" t="str">
-        <f>VLOOKUP(F90,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F90,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H90" s="14">
@@ -42881,7 +42881,7 @@
         <v>53</v>
       </c>
       <c r="G91" s="26" t="str">
-        <f>VLOOKUP(F91,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F91,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H91" s="14">
@@ -42964,7 +42964,7 @@
         <v>53</v>
       </c>
       <c r="G92" s="26" t="str">
-        <f>VLOOKUP(F92,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F92,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H92" s="14">
@@ -43051,7 +43051,7 @@
         <v>56</v>
       </c>
       <c r="G93" s="26" t="str">
-        <f>VLOOKUP(F93,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F93,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H93" s="14">
@@ -43138,7 +43138,7 @@
         <v>39</v>
       </c>
       <c r="G94" s="26" t="str">
-        <f>VLOOKUP(F94,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F94,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H94" s="14">
@@ -43225,7 +43225,7 @@
         <v>39</v>
       </c>
       <c r="G95" s="26" t="str">
-        <f>VLOOKUP(F95,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F95,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H95" s="14">
@@ -43304,7 +43304,7 @@
         <v>51</v>
       </c>
       <c r="G96" s="26" t="str">
-        <f>VLOOKUP(F96,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F96,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H96" s="14">
@@ -43391,7 +43391,7 @@
         <v>42</v>
       </c>
       <c r="G97" s="26" t="str">
-        <f>VLOOKUP(F97,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F97,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H97" s="14">
@@ -43478,8 +43478,8 @@
         <v>57</v>
       </c>
       <c r="G98" s="26" t="str">
-        <f>VLOOKUP(F98,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F98,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H98" s="14">
         <v>8654673.5800000001</v>
@@ -43569,7 +43569,7 @@
         <v>51</v>
       </c>
       <c r="G99" s="26" t="str">
-        <f>VLOOKUP(F99,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F99,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H99" s="14">
@@ -43648,7 +43648,7 @@
         <v>47</v>
       </c>
       <c r="G100" s="26" t="str">
-        <f>VLOOKUP(F100,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F100,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H100" s="14">
@@ -43735,7 +43735,7 @@
         <v>39</v>
       </c>
       <c r="G101" s="26" t="str">
-        <f>VLOOKUP(F101,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F101,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H101" s="14">
@@ -43814,7 +43814,7 @@
         <v>39</v>
       </c>
       <c r="G102" s="26" t="str">
-        <f>VLOOKUP(F102,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F102,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H102" s="14">
@@ -43901,7 +43901,7 @@
         <v>39</v>
       </c>
       <c r="G103" s="26" t="str">
-        <f>VLOOKUP(F103,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F103,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H103" s="14">
@@ -43988,7 +43988,7 @@
         <v>39</v>
       </c>
       <c r="G104" s="26" t="str">
-        <f>VLOOKUP(F104,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F104,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H104" s="14">
@@ -44075,7 +44075,7 @@
         <v>51</v>
       </c>
       <c r="G105" s="26" t="str">
-        <f>VLOOKUP(F105,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F105,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H105" s="14">
@@ -44162,7 +44162,7 @@
         <v>51</v>
       </c>
       <c r="G106" s="26" t="str">
-        <f>VLOOKUP(F106,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F106,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H106" s="14">
@@ -44241,7 +44241,7 @@
         <v>39</v>
       </c>
       <c r="G107" s="26" t="str">
-        <f>VLOOKUP(F107,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F107,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H107" s="14">
@@ -44332,7 +44332,7 @@
         <v>42</v>
       </c>
       <c r="G108" s="26" t="str">
-        <f>VLOOKUP(F108,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F108,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H108" s="14">
@@ -44419,7 +44419,7 @@
         <v>47</v>
       </c>
       <c r="G109" s="26" t="str">
-        <f>VLOOKUP(F109,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F109,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H109" s="14">
@@ -44514,7 +44514,7 @@
         <v>42</v>
       </c>
       <c r="G110" s="26" t="str">
-        <f>VLOOKUP(F110,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F110,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H110" s="14">
@@ -44593,7 +44593,7 @@
         <v>39</v>
       </c>
       <c r="G111" s="26" t="str">
-        <f>VLOOKUP(F111,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F111,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H111" s="14">
@@ -44672,7 +44672,7 @@
         <v>53</v>
       </c>
       <c r="G112" s="26" t="str">
-        <f>VLOOKUP(F112,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F112,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H112" s="14">
@@ -44759,7 +44759,7 @@
         <v>47</v>
       </c>
       <c r="G113" s="26" t="str">
-        <f>VLOOKUP(F113,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F113,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H113" s="14">
@@ -44838,7 +44838,7 @@
         <v>39</v>
       </c>
       <c r="G114" s="26" t="str">
-        <f>VLOOKUP(F114,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F114,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H114" s="14">
@@ -44917,7 +44917,7 @@
         <v>56</v>
       </c>
       <c r="G115" s="26" t="str">
-        <f>VLOOKUP(F115,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F115,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H115" s="14">
@@ -45004,7 +45004,7 @@
         <v>51</v>
       </c>
       <c r="G116" s="26" t="str">
-        <f>VLOOKUP(F116,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F116,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H116" s="14">
@@ -45095,7 +45095,7 @@
         <v>77</v>
       </c>
       <c r="G117" s="26" t="str">
-        <f>VLOOKUP(F117,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F117,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H117" s="14">
@@ -45178,7 +45178,7 @@
         <v>51</v>
       </c>
       <c r="G118" s="26" t="str">
-        <f>VLOOKUP(F118,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F118,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H118" s="14">
@@ -45257,7 +45257,7 @@
         <v>39</v>
       </c>
       <c r="G119" s="26" t="str">
-        <f>VLOOKUP(F119,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F119,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H119" s="14">
@@ -45344,7 +45344,7 @@
         <v>42</v>
       </c>
       <c r="G120" s="26" t="str">
-        <f>VLOOKUP(F120,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F120,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H120" s="14">
@@ -45437,7 +45437,7 @@
         <v>47</v>
       </c>
       <c r="G121" s="26" t="str">
-        <f>VLOOKUP(F121,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F121,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H121" s="14">
@@ -45530,7 +45530,7 @@
         <v>39</v>
       </c>
       <c r="G122" s="26" t="str">
-        <f>VLOOKUP(F122,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F122,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H122" s="14">
@@ -45617,7 +45617,7 @@
         <v>77</v>
       </c>
       <c r="G123" s="26" t="str">
-        <f>VLOOKUP(F123,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F123,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H123" s="14">
@@ -45696,7 +45696,7 @@
         <v>39</v>
       </c>
       <c r="G124" s="26" t="str">
-        <f>VLOOKUP(F124,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F124,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H124" s="14">
@@ -45787,7 +45787,7 @@
         <v>77</v>
       </c>
       <c r="G125" s="26" t="str">
-        <f>VLOOKUP(F125,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F125,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H125" s="14">
@@ -45878,7 +45878,7 @@
         <v>51</v>
       </c>
       <c r="G126" s="26" t="str">
-        <f>VLOOKUP(F126,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F126,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H126" s="14">
@@ -45965,7 +45965,7 @@
         <v>53</v>
       </c>
       <c r="G127" s="26" t="str">
-        <f>VLOOKUP(F127,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F127,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H127" s="14">
@@ -46044,7 +46044,7 @@
         <v>42</v>
       </c>
       <c r="G128" s="26" t="str">
-        <f>VLOOKUP(F128,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F128,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H128" s="14">
@@ -46131,7 +46131,7 @@
         <v>42</v>
       </c>
       <c r="G129" s="26" t="str">
-        <f>VLOOKUP(F129,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F129,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H129" s="14">
@@ -46218,7 +46218,7 @@
         <v>42</v>
       </c>
       <c r="G130" s="26" t="str">
-        <f>VLOOKUP(F130,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F130,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H130" s="14">
@@ -46305,7 +46305,7 @@
         <v>42</v>
       </c>
       <c r="G131" s="26" t="str">
-        <f>VLOOKUP(F131,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F131,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H131" s="14">
@@ -46388,7 +46388,7 @@
         <v>47</v>
       </c>
       <c r="G132" s="26" t="str">
-        <f>VLOOKUP(F132,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F132,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H132" s="14">
@@ -46479,7 +46479,7 @@
         <v>39</v>
       </c>
       <c r="G133" s="26" t="str">
-        <f>VLOOKUP(F133,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F133,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H133" s="14">
@@ -46570,7 +46570,7 @@
         <v>56</v>
       </c>
       <c r="G134" s="26" t="str">
-        <f>VLOOKUP(F134,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F134,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H134" s="14">
@@ -46657,7 +46657,7 @@
         <v>39</v>
       </c>
       <c r="G135" s="26" t="str">
-        <f>VLOOKUP(F135,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F135,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H135" s="14">
@@ -46748,7 +46748,7 @@
         <v>42</v>
       </c>
       <c r="G136" s="26" t="str">
-        <f>VLOOKUP(F136,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F136,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H136" s="14">
@@ -46837,7 +46837,7 @@
         <v>39</v>
       </c>
       <c r="G137" s="26" t="str">
-        <f>VLOOKUP(F137,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F137,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H137" s="14">
@@ -46928,7 +46928,7 @@
         <v>53</v>
       </c>
       <c r="G138" s="26" t="str">
-        <f>VLOOKUP(F138,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F138,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H138" s="14">
@@ -47007,7 +47007,7 @@
         <v>42</v>
       </c>
       <c r="G139" s="26" t="str">
-        <f>VLOOKUP(F139,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F139,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H139" s="14">
@@ -47090,7 +47090,7 @@
         <v>39</v>
       </c>
       <c r="G140" s="26" t="str">
-        <f>VLOOKUP(F140,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F140,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H140" s="14">
@@ -47169,7 +47169,7 @@
         <v>53</v>
       </c>
       <c r="G141" s="26" t="str">
-        <f>VLOOKUP(F141,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F141,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H141" s="14">
@@ -47248,7 +47248,7 @@
         <v>42</v>
       </c>
       <c r="G142" s="26" t="str">
-        <f>VLOOKUP(F142,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F142,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H142" s="14">
@@ -47335,7 +47335,7 @@
         <v>53</v>
       </c>
       <c r="G143" s="26" t="str">
-        <f>VLOOKUP(F143,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F143,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H143" s="14">
@@ -47422,7 +47422,7 @@
         <v>39</v>
       </c>
       <c r="G144" s="26" t="str">
-        <f>VLOOKUP(F144,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F144,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H144" s="14">
@@ -47513,7 +47513,7 @@
         <v>77</v>
       </c>
       <c r="G145" s="26" t="str">
-        <f>VLOOKUP(F145,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F145,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H145" s="14">
@@ -47592,7 +47592,7 @@
         <v>39</v>
       </c>
       <c r="G146" s="26" t="str">
-        <f>VLOOKUP(F146,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F146,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H146" s="14">
@@ -47671,7 +47671,7 @@
         <v>58</v>
       </c>
       <c r="G147" s="26" t="str">
-        <f>VLOOKUP(F147,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F147,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>16 Opole Province</v>
       </c>
       <c r="H147" s="14">
@@ -47758,7 +47758,7 @@
         <v>58</v>
       </c>
       <c r="G148" s="26" t="str">
-        <f>VLOOKUP(F148,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F148,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>16 Opole Province</v>
       </c>
       <c r="H148" s="14">
@@ -47845,7 +47845,7 @@
         <v>47</v>
       </c>
       <c r="G149" s="26" t="str">
-        <f>VLOOKUP(F149,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F149,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H149" s="14">
@@ -47932,7 +47932,7 @@
         <v>53</v>
       </c>
       <c r="G150" s="26" t="str">
-        <f>VLOOKUP(F150,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F150,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H150" s="14">
@@ -48019,7 +48019,7 @@
         <v>77</v>
       </c>
       <c r="G151" s="26" t="str">
-        <f>VLOOKUP(F151,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F151,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H151" s="14">
@@ -48102,7 +48102,7 @@
         <v>58</v>
       </c>
       <c r="G152" s="26" t="str">
-        <f>VLOOKUP(F152,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F152,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>16 Opole Province</v>
       </c>
       <c r="H152" s="14">
@@ -48189,7 +48189,7 @@
         <v>58</v>
       </c>
       <c r="G153" s="26" t="str">
-        <f>VLOOKUP(F153,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F153,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>16 Opole Province</v>
       </c>
       <c r="H153" s="14">
@@ -48280,7 +48280,7 @@
         <v>77</v>
       </c>
       <c r="G154" s="26" t="str">
-        <f>VLOOKUP(F154,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F154,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H154" s="14">
@@ -48371,7 +48371,7 @@
         <v>77</v>
       </c>
       <c r="G155" s="26" t="str">
-        <f>VLOOKUP(F155,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F155,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H155" s="14">
@@ -48458,7 +48458,7 @@
         <v>77</v>
       </c>
       <c r="G156" s="26" t="str">
-        <f>VLOOKUP(F156,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F156,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H156" s="14">
@@ -48545,7 +48545,7 @@
         <v>69</v>
       </c>
       <c r="G157" s="26" t="str">
-        <f>VLOOKUP(F157,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F157,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H157" s="14">
@@ -48624,8 +48624,8 @@
         <v>57</v>
       </c>
       <c r="G158" s="26" t="str">
-        <f>VLOOKUP(F158,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F158,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H158" s="14">
         <v>8629281.3900000006</v>
@@ -48703,7 +48703,7 @@
         <v>69</v>
       </c>
       <c r="G159" s="26" t="str">
-        <f>VLOOKUP(F159,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F159,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H159" s="14">
@@ -48794,7 +48794,7 @@
         <v>69</v>
       </c>
       <c r="G160" s="26" t="str">
-        <f>VLOOKUP(F160,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F160,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H160" s="14">
@@ -48877,7 +48877,7 @@
         <v>51</v>
       </c>
       <c r="G161" s="26" t="str">
-        <f>VLOOKUP(F161,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F161,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H161" s="14">
@@ -48956,7 +48956,7 @@
         <v>53</v>
       </c>
       <c r="G162" s="26" t="str">
-        <f>VLOOKUP(F162,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F162,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H162" s="14">
@@ -49043,7 +49043,7 @@
         <v>69</v>
       </c>
       <c r="G163" s="26" t="str">
-        <f>VLOOKUP(F163,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F163,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H163" s="14">
@@ -49126,7 +49126,7 @@
         <v>77</v>
       </c>
       <c r="G164" s="26" t="str">
-        <f>VLOOKUP(F164,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F164,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H164" s="14">
@@ -49213,7 +49213,7 @@
         <v>42</v>
       </c>
       <c r="G165" s="26" t="str">
-        <f>VLOOKUP(F165,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F165,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H165" s="14">
@@ -49292,7 +49292,7 @@
         <v>69</v>
       </c>
       <c r="G166" s="26" t="str">
-        <f>VLOOKUP(F166,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F166,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H166" s="14">
@@ -49371,7 +49371,7 @@
         <v>53</v>
       </c>
       <c r="G167" s="26" t="str">
-        <f>VLOOKUP(F167,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F167,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H167" s="14">
@@ -49458,7 +49458,7 @@
         <v>39</v>
       </c>
       <c r="G168" s="26" t="str">
-        <f>VLOOKUP(F168,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F168,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H168" s="14">
@@ -49545,8 +49545,8 @@
         <v>57</v>
       </c>
       <c r="G169" s="26" t="str">
-        <f>VLOOKUP(F169,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F169,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H169" s="14">
         <v>8626377.6899999995</v>
@@ -49624,7 +49624,7 @@
         <v>69</v>
       </c>
       <c r="G170" s="26" t="str">
-        <f>VLOOKUP(F170,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F170,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H170" s="14">
@@ -49703,7 +49703,7 @@
         <v>69</v>
       </c>
       <c r="G171" s="26" t="str">
-        <f>VLOOKUP(F171,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F171,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H171" s="14">
@@ -49782,7 +49782,7 @@
         <v>42</v>
       </c>
       <c r="G172" s="26" t="str">
-        <f>VLOOKUP(F172,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F172,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H172" s="14">
@@ -49869,7 +49869,7 @@
         <v>77</v>
       </c>
       <c r="G173" s="26" t="str">
-        <f>VLOOKUP(F173,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F173,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H173" s="14">
@@ -49956,7 +49956,7 @@
         <v>56</v>
       </c>
       <c r="G174" s="26" t="str">
-        <f>VLOOKUP(F174,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F174,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H174" s="14">
@@ -50039,7 +50039,7 @@
         <v>42</v>
       </c>
       <c r="G175" s="26" t="str">
-        <f>VLOOKUP(F175,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F175,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H175" s="14">
@@ -50126,8 +50126,8 @@
         <v>57</v>
       </c>
       <c r="G176" s="26" t="str">
-        <f>VLOOKUP(F176,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F176,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H176" s="14">
         <v>8623740.8399999999</v>
@@ -50219,7 +50219,7 @@
         <v>39</v>
       </c>
       <c r="G177" s="26" t="str">
-        <f>VLOOKUP(F177,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F177,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H177" s="14">
@@ -50298,7 +50298,7 @@
         <v>69</v>
       </c>
       <c r="G178" s="26" t="str">
-        <f>VLOOKUP(F178,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F178,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H178" s="14">
@@ -50385,7 +50385,7 @@
         <v>39</v>
       </c>
       <c r="G179" s="26" t="str">
-        <f>VLOOKUP(F179,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F179,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H179" s="14">
@@ -50472,7 +50472,7 @@
         <v>69</v>
       </c>
       <c r="G180" s="26" t="str">
-        <f>VLOOKUP(F180,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F180,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H180" s="14">
@@ -50559,7 +50559,7 @@
         <v>47</v>
       </c>
       <c r="G181" s="26" t="str">
-        <f>VLOOKUP(F181,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F181,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H181" s="14">
@@ -50646,7 +50646,7 @@
         <v>42</v>
       </c>
       <c r="G182" s="26" t="str">
-        <f>VLOOKUP(F182,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F182,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H182" s="14">
@@ -50725,7 +50725,7 @@
         <v>39</v>
       </c>
       <c r="G183" s="26" t="str">
-        <f>VLOOKUP(F183,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F183,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H183" s="14">
@@ -50812,7 +50812,7 @@
         <v>47</v>
       </c>
       <c r="G184" s="26" t="str">
-        <f>VLOOKUP(F184,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F184,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H184" s="14">
@@ -50903,7 +50903,7 @@
         <v>69</v>
       </c>
       <c r="G185" s="26" t="str">
-        <f>VLOOKUP(F185,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F185,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H185" s="14">
@@ -50990,7 +50990,7 @@
         <v>53</v>
       </c>
       <c r="G186" s="26" t="str">
-        <f>VLOOKUP(F186,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F186,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H186" s="14">
@@ -51081,7 +51081,7 @@
         <v>51</v>
       </c>
       <c r="G187" s="26" t="str">
-        <f>VLOOKUP(F187,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F187,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H187" s="14">
@@ -51164,7 +51164,7 @@
         <v>51</v>
       </c>
       <c r="G188" s="26" t="str">
-        <f>VLOOKUP(F188,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F188,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H188" s="14">
@@ -51247,8 +51247,8 @@
         <v>57</v>
       </c>
       <c r="G189" s="26" t="str">
-        <f>VLOOKUP(F189,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F189,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H189" s="14">
         <v>8618798.9199999999</v>
@@ -51326,7 +51326,7 @@
         <v>39</v>
       </c>
       <c r="G190" s="26" t="str">
-        <f>VLOOKUP(F190,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F190,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H190" s="14">
@@ -51405,7 +51405,7 @@
         <v>69</v>
       </c>
       <c r="G191" s="26" t="str">
-        <f>VLOOKUP(F191,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F191,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H191" s="14">
@@ -51488,7 +51488,7 @@
         <v>69</v>
       </c>
       <c r="G192" s="26" t="str">
-        <f>VLOOKUP(F192,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F192,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H192" s="14">
@@ -51567,7 +51567,7 @@
         <v>39</v>
       </c>
       <c r="G193" s="26" t="str">
-        <f>VLOOKUP(F193,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F193,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H193" s="14">
@@ -51654,7 +51654,7 @@
         <v>42</v>
       </c>
       <c r="G194" s="26" t="str">
-        <f>VLOOKUP(F194,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F194,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H194" s="14">
@@ -51741,7 +51741,7 @@
         <v>69</v>
       </c>
       <c r="G195" s="26" t="str">
-        <f>VLOOKUP(F195,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F195,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H195" s="14">
@@ -51828,7 +51828,7 @@
         <v>77</v>
       </c>
       <c r="G196" s="26" t="str">
-        <f>VLOOKUP(F196,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F196,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H196" s="14">
@@ -51919,7 +51919,7 @@
         <v>69</v>
       </c>
       <c r="G197" s="26" t="str">
-        <f>VLOOKUP(F197,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F197,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H197" s="14">
@@ -51998,7 +51998,7 @@
         <v>65</v>
       </c>
       <c r="G198" s="26" t="str">
-        <f>VLOOKUP(F198,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F198,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H198" s="14">
@@ -52077,7 +52077,7 @@
         <v>65</v>
       </c>
       <c r="G199" s="26" t="str">
-        <f>VLOOKUP(F199,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F199,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H199" s="14">
@@ -52168,7 +52168,7 @@
         <v>69</v>
       </c>
       <c r="G200" s="26" t="str">
-        <f>VLOOKUP(F200,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F200,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H200" s="14">
@@ -52255,7 +52255,7 @@
         <v>69</v>
       </c>
       <c r="G201" s="26" t="str">
-        <f>VLOOKUP(F201,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F201,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H201" s="14">
@@ -52342,7 +52342,7 @@
         <v>47</v>
       </c>
       <c r="G202" s="26" t="str">
-        <f>VLOOKUP(F202,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F202,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H202" s="14">
@@ -52429,7 +52429,7 @@
         <v>39</v>
       </c>
       <c r="G203" s="26" t="str">
-        <f>VLOOKUP(F203,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F203,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H203" s="14">
@@ -52516,7 +52516,7 @@
         <v>69</v>
       </c>
       <c r="G204" s="26" t="str">
-        <f>VLOOKUP(F204,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F204,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H204" s="14">
@@ -52599,7 +52599,7 @@
         <v>77</v>
       </c>
       <c r="G205" s="26" t="str">
-        <f>VLOOKUP(F205,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F205,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H205" s="14">
@@ -52690,7 +52690,7 @@
         <v>42</v>
       </c>
       <c r="G206" s="26" t="str">
-        <f>VLOOKUP(F206,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F206,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H206" s="14">
@@ -52769,7 +52769,7 @@
         <v>39</v>
       </c>
       <c r="G207" s="26" t="str">
-        <f>VLOOKUP(F207,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F207,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H207" s="14">
@@ -52848,7 +52848,7 @@
         <v>65</v>
       </c>
       <c r="G208" s="26" t="str">
-        <f>VLOOKUP(F208,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F208,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H208" s="14">
@@ -52931,8 +52931,8 @@
         <v>57</v>
       </c>
       <c r="G209" s="26" t="str">
-        <f>VLOOKUP(F209,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F209,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H209" s="14">
         <v>8611893</v>
@@ -53010,7 +53010,7 @@
         <v>39</v>
       </c>
       <c r="G210" s="26" t="str">
-        <f>VLOOKUP(F210,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F210,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H210" s="14">
@@ -53101,7 +53101,7 @@
         <v>39</v>
       </c>
       <c r="G211" s="26" t="str">
-        <f>VLOOKUP(F211,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F211,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H211" s="14">
@@ -53188,7 +53188,7 @@
         <v>47</v>
       </c>
       <c r="G212" s="26" t="str">
-        <f>VLOOKUP(F212,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F212,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H212" s="14">
@@ -53267,7 +53267,7 @@
         <v>65</v>
       </c>
       <c r="G213" s="26" t="str">
-        <f>VLOOKUP(F213,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F213,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H213" s="14">
@@ -53362,7 +53362,7 @@
         <v>51</v>
       </c>
       <c r="G214" s="26" t="str">
-        <f>VLOOKUP(F214,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F214,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H214" s="14">
@@ -53441,7 +53441,7 @@
         <v>39</v>
       </c>
       <c r="G215" s="26" t="str">
-        <f>VLOOKUP(F215,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F215,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H215" s="14">
@@ -53524,7 +53524,7 @@
         <v>77</v>
       </c>
       <c r="G216" s="26" t="str">
-        <f>VLOOKUP(F216,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F216,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H216" s="14">
@@ -53615,7 +53615,7 @@
         <v>42</v>
       </c>
       <c r="G217" s="26" t="str">
-        <f>VLOOKUP(F217,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F217,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H217" s="14">
@@ -53706,7 +53706,7 @@
         <v>69</v>
       </c>
       <c r="G218" s="26" t="str">
-        <f>VLOOKUP(F218,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F218,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H218" s="14">
@@ -53793,7 +53793,7 @@
         <v>69</v>
       </c>
       <c r="G219" s="26" t="str">
-        <f>VLOOKUP(F219,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F219,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>18 Podkarpackie Province</v>
       </c>
       <c r="H219" s="14">
@@ -53884,7 +53884,7 @@
         <v>39</v>
       </c>
       <c r="G220" s="26" t="str">
-        <f>VLOOKUP(F220,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F220,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H220" s="14">
@@ -53977,7 +53977,7 @@
         <v>77</v>
       </c>
       <c r="G221" s="26" t="str">
-        <f>VLOOKUP(F221,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F221,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H221" s="14">
@@ -54062,7 +54062,7 @@
         <v>64</v>
       </c>
       <c r="G222" s="26" t="str">
-        <f>VLOOKUP(F222,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F222,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H222" s="14">
@@ -54145,7 +54145,7 @@
         <v>39</v>
       </c>
       <c r="G223" s="26" t="str">
-        <f>VLOOKUP(F223,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F223,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H223" s="14">
@@ -54236,7 +54236,7 @@
         <v>65</v>
       </c>
       <c r="G224" s="26" t="str">
-        <f>VLOOKUP(F224,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F224,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H224" s="14">
@@ -54327,7 +54327,7 @@
         <v>64</v>
       </c>
       <c r="G225" s="26" t="str">
-        <f>VLOOKUP(F225,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F225,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H225" s="14">
@@ -54414,7 +54414,7 @@
         <v>64</v>
       </c>
       <c r="G226" s="26" t="str">
-        <f>VLOOKUP(F226,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F226,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H226" s="14">
@@ -54501,7 +54501,7 @@
         <v>47</v>
       </c>
       <c r="G227" s="26" t="str">
-        <f>VLOOKUP(F227,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F227,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H227" s="14">
@@ -54592,7 +54592,7 @@
         <v>56</v>
       </c>
       <c r="G228" s="26" t="str">
-        <f>VLOOKUP(F228,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F228,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H228" s="14">
@@ -54675,7 +54675,7 @@
         <v>39</v>
       </c>
       <c r="G229" s="26" t="str">
-        <f>VLOOKUP(F229,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F229,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H229" s="14">
@@ -54754,7 +54754,7 @@
         <v>64</v>
       </c>
       <c r="G230" s="26" t="str">
-        <f>VLOOKUP(F230,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F230,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H230" s="14">
@@ -54841,7 +54841,7 @@
         <v>39</v>
       </c>
       <c r="G231" s="26" t="str">
-        <f>VLOOKUP(F231,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F231,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H231" s="14">
@@ -54928,7 +54928,7 @@
         <v>64</v>
       </c>
       <c r="G232" s="26" t="str">
-        <f>VLOOKUP(F232,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F232,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H232" s="14">
@@ -55015,7 +55015,7 @@
         <v>51</v>
       </c>
       <c r="G233" s="26" t="str">
-        <f>VLOOKUP(F233,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F233,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H233" s="14">
@@ -55094,7 +55094,7 @@
         <v>47</v>
       </c>
       <c r="G234" s="26" t="str">
-        <f>VLOOKUP(F234,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F234,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H234" s="14">
@@ -55185,7 +55185,7 @@
         <v>65</v>
       </c>
       <c r="G235" s="26" t="str">
-        <f>VLOOKUP(F235,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F235,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H235" s="14">
@@ -55272,7 +55272,7 @@
         <v>39</v>
       </c>
       <c r="G236" s="26" t="str">
-        <f>VLOOKUP(F236,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F236,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H236" s="14">
@@ -55361,7 +55361,7 @@
         <v>77</v>
       </c>
       <c r="G237" s="26" t="str">
-        <f>VLOOKUP(F237,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F237,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H237" s="14">
@@ -55448,7 +55448,7 @@
         <v>64</v>
       </c>
       <c r="G238" s="26" t="str">
-        <f>VLOOKUP(F238,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F238,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H238" s="14">
@@ -55531,7 +55531,7 @@
         <v>77</v>
       </c>
       <c r="G239" s="26" t="str">
-        <f>VLOOKUP(F239,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F239,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>04 Kuyavian-Pomeranian Province</v>
       </c>
       <c r="H239" s="14">
@@ -55618,7 +55618,7 @@
         <v>39</v>
       </c>
       <c r="G240" s="26" t="str">
-        <f>VLOOKUP(F240,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F240,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H240" s="14">
@@ -55705,7 +55705,7 @@
         <v>39</v>
       </c>
       <c r="G241" s="26" t="str">
-        <f>VLOOKUP(F241,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F241,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H241" s="14">
@@ -55792,7 +55792,7 @@
         <v>56</v>
       </c>
       <c r="G242" s="26" t="str">
-        <f>VLOOKUP(F242,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F242,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H242" s="14">
@@ -55879,7 +55879,7 @@
         <v>42</v>
       </c>
       <c r="G243" s="26" t="str">
-        <f>VLOOKUP(F243,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F243,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H243" s="14">
@@ -55966,7 +55966,7 @@
         <v>47</v>
       </c>
       <c r="G244" s="26" t="str">
-        <f>VLOOKUP(F244,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F244,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H244" s="14">
@@ -56057,7 +56057,7 @@
         <v>39</v>
       </c>
       <c r="G245" s="26" t="str">
-        <f>VLOOKUP(F245,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F245,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H245" s="14">
@@ -56144,7 +56144,7 @@
         <v>64</v>
       </c>
       <c r="G246" s="26" t="str">
-        <f>VLOOKUP(F246,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F246,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H246" s="14">
@@ -56231,7 +56231,7 @@
         <v>64</v>
       </c>
       <c r="G247" s="26" t="str">
-        <f>VLOOKUP(F247,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F247,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H247" s="14">
@@ -56318,7 +56318,7 @@
         <v>64</v>
       </c>
       <c r="G248" s="26" t="str">
-        <f>VLOOKUP(F248,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F248,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H248" s="14">
@@ -56405,7 +56405,7 @@
         <v>39</v>
       </c>
       <c r="G249" s="26" t="str">
-        <f>VLOOKUP(F249,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F249,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H249" s="14">
@@ -56492,7 +56492,7 @@
         <v>56</v>
       </c>
       <c r="G250" s="26" t="str">
-        <f>VLOOKUP(F250,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F250,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H250" s="14">
@@ -56583,7 +56583,7 @@
         <v>64</v>
       </c>
       <c r="G251" s="26" t="str">
-        <f>VLOOKUP(F251,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F251,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>20 Podlasie Province</v>
       </c>
       <c r="H251" s="14">
@@ -56670,7 +56670,7 @@
         <v>39</v>
       </c>
       <c r="G252" s="26" t="str">
-        <f>VLOOKUP(F252,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F252,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H252" s="14">
@@ -56757,7 +56757,7 @@
         <v>42</v>
       </c>
       <c r="G253" s="26" t="str">
-        <f>VLOOKUP(F253,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F253,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H253" s="14">
@@ -56836,7 +56836,7 @@
         <v>39</v>
       </c>
       <c r="G254" s="26" t="str">
-        <f>VLOOKUP(F254,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F254,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H254" s="14">
@@ -56923,7 +56923,7 @@
         <v>39</v>
       </c>
       <c r="G255" s="26" t="str">
-        <f>VLOOKUP(F255,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F255,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H255" s="14">
@@ -57010,7 +57010,7 @@
         <v>42</v>
       </c>
       <c r="G256" s="26" t="str">
-        <f>VLOOKUP(F256,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F256,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H256" s="14">
@@ -57101,7 +57101,7 @@
         <v>46</v>
       </c>
       <c r="G257" s="26" t="str">
-        <f>VLOOKUP(F257,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F257,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H257" s="14">
@@ -57192,7 +57192,7 @@
         <v>46</v>
       </c>
       <c r="G258" s="26" t="str">
-        <f>VLOOKUP(F258,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F258,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H258" s="14">
@@ -57271,7 +57271,7 @@
         <v>46</v>
       </c>
       <c r="G259" s="26" t="str">
-        <f>VLOOKUP(F259,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F259,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H259" s="14">
@@ -57358,7 +57358,7 @@
         <v>42</v>
       </c>
       <c r="G260" s="26" t="str">
-        <f>VLOOKUP(F260,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F260,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H260" s="14">
@@ -57447,7 +57447,7 @@
         <v>49</v>
       </c>
       <c r="G261" s="26" t="str">
-        <f>VLOOKUP(F261,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F261,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>06 Lublin Province</v>
       </c>
       <c r="H261" s="14">
@@ -57534,7 +57534,7 @@
         <v>39</v>
       </c>
       <c r="G262" s="26" t="str">
-        <f>VLOOKUP(F262,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F262,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H262" s="14">
@@ -57621,7 +57621,7 @@
         <v>47</v>
       </c>
       <c r="G263" s="26" t="str">
-        <f>VLOOKUP(F263,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F263,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H263" s="14">
@@ -57708,7 +57708,7 @@
         <v>46</v>
       </c>
       <c r="G264" s="26" t="str">
-        <f>VLOOKUP(F264,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F264,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H264" s="14">
@@ -57795,8 +57795,8 @@
         <v>57</v>
       </c>
       <c r="G265" s="26" t="str">
-        <f>VLOOKUP(F265,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F265,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H265" s="14">
         <v>8587517.8399999999</v>
@@ -57882,7 +57882,7 @@
         <v>46</v>
       </c>
       <c r="G266" s="26" t="str">
-        <f>VLOOKUP(F266,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F266,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H266" s="14">
@@ -57973,7 +57973,7 @@
         <v>42</v>
       </c>
       <c r="G267" s="26" t="str">
-        <f>VLOOKUP(F267,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F267,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H267" s="14">
@@ -58060,7 +58060,7 @@
         <v>42</v>
       </c>
       <c r="G268" s="26" t="str">
-        <f>VLOOKUP(F268,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F268,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H268" s="14">
@@ -58151,7 +58151,7 @@
         <v>46</v>
       </c>
       <c r="G269" s="26" t="str">
-        <f>VLOOKUP(F269,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F269,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H269" s="14">
@@ -58238,7 +58238,7 @@
         <v>39</v>
       </c>
       <c r="G270" s="26" t="str">
-        <f>VLOOKUP(F270,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F270,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H270" s="14">
@@ -58317,7 +58317,7 @@
         <v>56</v>
       </c>
       <c r="G271" s="26" t="str">
-        <f>VLOOKUP(F271,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F271,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H271" s="14">
@@ -58412,7 +58412,7 @@
         <v>65</v>
       </c>
       <c r="G272" s="26" t="str">
-        <f>VLOOKUP(F272,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F272,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H272" s="14">
@@ -58495,7 +58495,7 @@
         <v>39</v>
       </c>
       <c r="G273" s="26" t="str">
-        <f>VLOOKUP(F273,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F273,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H273" s="14">
@@ -58582,7 +58582,7 @@
         <v>39</v>
       </c>
       <c r="G274" s="26" t="str">
-        <f>VLOOKUP(F274,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F274,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H274" s="14">
@@ -58673,7 +58673,7 @@
         <v>46</v>
       </c>
       <c r="G275" s="26" t="str">
-        <f>VLOOKUP(F275,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F275,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H275" s="14">
@@ -58760,7 +58760,7 @@
         <v>65</v>
       </c>
       <c r="G276" s="26" t="str">
-        <f>VLOOKUP(F276,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F276,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H276" s="14">
@@ -58839,7 +58839,7 @@
         <v>46</v>
       </c>
       <c r="G277" s="26" t="str">
-        <f>VLOOKUP(F277,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F277,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H277" s="14">
@@ -58918,7 +58918,7 @@
         <v>42</v>
       </c>
       <c r="G278" s="26" t="str">
-        <f>VLOOKUP(F278,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F278,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H278" s="14">
@@ -59009,7 +59009,7 @@
         <v>46</v>
       </c>
       <c r="G279" s="26" t="str">
-        <f>VLOOKUP(F279,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F279,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H279" s="14">
@@ -59088,7 +59088,7 @@
         <v>53</v>
       </c>
       <c r="G280" s="26" t="str">
-        <f>VLOOKUP(F280,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F280,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>12 Lesser Poland Province</v>
       </c>
       <c r="H280" s="14">
@@ -59171,7 +59171,7 @@
         <v>49</v>
       </c>
       <c r="G281" s="26" t="str">
-        <f>VLOOKUP(F281,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F281,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>06 Lublin Province</v>
       </c>
       <c r="H281" s="14">
@@ -59258,7 +59258,7 @@
         <v>39</v>
       </c>
       <c r="G282" s="26" t="str">
-        <f>VLOOKUP(F282,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F282,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H282" s="14">
@@ -59337,7 +59337,7 @@
         <v>46</v>
       </c>
       <c r="G283" s="26" t="str">
-        <f>VLOOKUP(F283,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F283,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H283" s="14">
@@ -59424,7 +59424,7 @@
         <v>42</v>
       </c>
       <c r="G284" s="26" t="str">
-        <f>VLOOKUP(F284,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F284,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H284" s="14">
@@ -59511,7 +59511,7 @@
         <v>49</v>
       </c>
       <c r="G285" s="26" t="str">
-        <f>VLOOKUP(F285,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F285,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>06 Lublin Province</v>
       </c>
       <c r="H285" s="14">
@@ -59590,7 +59590,7 @@
         <v>39</v>
       </c>
       <c r="G286" s="26" t="str">
-        <f>VLOOKUP(F286,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F286,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H286" s="14">
@@ -59677,7 +59677,7 @@
         <v>46</v>
       </c>
       <c r="G287" s="26" t="str">
-        <f>VLOOKUP(F287,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F287,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H287" s="14">
@@ -59760,8 +59760,8 @@
         <v>57</v>
       </c>
       <c r="G288" s="26" t="str">
-        <f>VLOOKUP(F288,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F288,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H288" s="14">
         <v>8580338.3699999992</v>
@@ -59843,7 +59843,7 @@
         <v>65</v>
       </c>
       <c r="G289" s="26" t="str">
-        <f>VLOOKUP(F289,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F289,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H289" s="14">
@@ -59930,7 +59930,7 @@
         <v>46</v>
       </c>
       <c r="G290" s="26" t="str">
-        <f>VLOOKUP(F290,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F290,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H290" s="14">
@@ -60017,7 +60017,7 @@
         <v>42</v>
       </c>
       <c r="G291" s="26" t="str">
-        <f>VLOOKUP(F291,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F291,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H291" s="14">
@@ -60100,7 +60100,7 @@
         <v>49</v>
       </c>
       <c r="G292" s="26" t="str">
-        <f>VLOOKUP(F292,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F292,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>06 Lublin Province</v>
       </c>
       <c r="H292" s="14">
@@ -60183,7 +60183,7 @@
         <v>46</v>
       </c>
       <c r="G293" s="26" t="str">
-        <f>VLOOKUP(F293,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F293,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H293" s="14">
@@ -60270,7 +60270,7 @@
         <v>65</v>
       </c>
       <c r="G294" s="26" t="str">
-        <f>VLOOKUP(F294,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F294,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H294" s="14">
@@ -60357,7 +60357,7 @@
         <v>46</v>
       </c>
       <c r="G295" s="26" t="str">
-        <f>VLOOKUP(F295,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F295,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H295" s="14">
@@ -60444,7 +60444,7 @@
         <v>39</v>
       </c>
       <c r="G296" s="26" t="str">
-        <f>VLOOKUP(F296,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F296,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H296" s="14">
@@ -60531,7 +60531,7 @@
         <v>39</v>
       </c>
       <c r="G297" s="26" t="str">
-        <f>VLOOKUP(F297,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F297,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H297" s="14">
@@ -60618,7 +60618,7 @@
         <v>39</v>
       </c>
       <c r="G298" s="26" t="str">
-        <f>VLOOKUP(F298,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F298,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H298" s="14">
@@ -60697,7 +60697,7 @@
         <v>39</v>
       </c>
       <c r="G299" s="26" t="str">
-        <f>VLOOKUP(F299,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F299,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H299" s="14">
@@ -60780,7 +60780,7 @@
         <v>65</v>
       </c>
       <c r="G300" s="26" t="str">
-        <f>VLOOKUP(F300,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F300,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H300" s="14">
@@ -60863,7 +60863,7 @@
         <v>49</v>
       </c>
       <c r="G301" s="26" t="str">
-        <f>VLOOKUP(F301,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F301,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>06 Lublin Province</v>
       </c>
       <c r="H301" s="14">
@@ -60950,7 +60950,7 @@
         <v>46</v>
       </c>
       <c r="G302" s="26" t="str">
-        <f>VLOOKUP(F302,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F302,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H302" s="14">
@@ -61029,7 +61029,7 @@
         <v>56</v>
       </c>
       <c r="G303" s="26" t="str">
-        <f>VLOOKUP(F303,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F303,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H303" s="14">
@@ -61116,7 +61116,7 @@
         <v>49</v>
       </c>
       <c r="G304" s="26" t="str">
-        <f>VLOOKUP(F304,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F304,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>06 Lublin Province</v>
       </c>
       <c r="H304" s="14">
@@ -61203,7 +61203,7 @@
         <v>39</v>
       </c>
       <c r="G305" s="26" t="str">
-        <f>VLOOKUP(F305,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F305,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H305" s="14">
@@ -61294,7 +61294,7 @@
         <v>46</v>
       </c>
       <c r="G306" s="26" t="str">
-        <f>VLOOKUP(F306,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F306,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H306" s="14">
@@ -61385,7 +61385,7 @@
         <v>46</v>
       </c>
       <c r="G307" s="26" t="str">
-        <f>VLOOKUP(F307,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F307,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H307" s="14">
@@ -61472,7 +61472,7 @@
         <v>46</v>
       </c>
       <c r="G308" s="26" t="str">
-        <f>VLOOKUP(F308,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F308,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H308" s="14">
@@ -61559,7 +61559,7 @@
         <v>39</v>
       </c>
       <c r="G309" s="26" t="str">
-        <f>VLOOKUP(F309,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F309,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H309" s="14">
@@ -61646,7 +61646,7 @@
         <v>47</v>
       </c>
       <c r="G310" s="26" t="str">
-        <f>VLOOKUP(F310,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F310,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H310" s="14">
@@ -61733,7 +61733,7 @@
         <v>51</v>
       </c>
       <c r="G311" s="26" t="str">
-        <f>VLOOKUP(F311,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F311,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H311" s="14">
@@ -61812,7 +61812,7 @@
         <v>39</v>
       </c>
       <c r="G312" s="26" t="str">
-        <f>VLOOKUP(F312,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F312,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H312" s="14">
@@ -61899,7 +61899,7 @@
         <v>42</v>
       </c>
       <c r="G313" s="26" t="str">
-        <f>VLOOKUP(F313,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F313,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H313" s="14">
@@ -61986,7 +61986,7 @@
         <v>42</v>
       </c>
       <c r="G314" s="26" t="str">
-        <f>VLOOKUP(F314,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F314,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H314" s="14">
@@ -62073,7 +62073,7 @@
         <v>47</v>
       </c>
       <c r="G315" s="26" t="str">
-        <f>VLOOKUP(F315,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F315,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H315" s="14">
@@ -62160,7 +62160,7 @@
         <v>42</v>
       </c>
       <c r="G316" s="26" t="str">
-        <f>VLOOKUP(F316,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F316,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H316" s="14">
@@ -62239,8 +62239,8 @@
         <v>57</v>
       </c>
       <c r="G317" s="26" t="str">
-        <f>VLOOKUP(F317,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F317,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H317" s="14">
         <v>8563135.1199999992</v>
@@ -62326,7 +62326,7 @@
         <v>49</v>
       </c>
       <c r="G318" s="26" t="str">
-        <f>VLOOKUP(F318,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F318,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>06 Lublin Province</v>
       </c>
       <c r="H318" s="14">
@@ -62413,7 +62413,7 @@
         <v>51</v>
       </c>
       <c r="G319" s="26" t="str">
-        <f>VLOOKUP(F319,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F319,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H319" s="14">
@@ -62492,7 +62492,7 @@
         <v>39</v>
       </c>
       <c r="G320" s="26" t="str">
-        <f>VLOOKUP(F320,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F320,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H320" s="14">
@@ -62579,7 +62579,7 @@
         <v>46</v>
       </c>
       <c r="G321" s="26" t="str">
-        <f>VLOOKUP(F321,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F321,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H321" s="14">
@@ -62666,7 +62666,7 @@
         <v>39</v>
       </c>
       <c r="G322" s="26" t="str">
-        <f>VLOOKUP(F322,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F322,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H322" s="14">
@@ -62757,7 +62757,7 @@
         <v>49</v>
       </c>
       <c r="G323" s="26" t="str">
-        <f>VLOOKUP(F323,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F323,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>06 Lublin Province</v>
       </c>
       <c r="H323" s="14">
@@ -62847,9 +62847,9 @@
       <c r="F324" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G324" s="26" t="e">
-        <f>VLOOKUP(F324,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G324" s="26" t="str">
+        <f>VLOOKUP(F324,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H324" s="14">
         <v>8560736.7400000002</v>
@@ -62939,7 +62939,7 @@
         <v>39</v>
       </c>
       <c r="G325" s="26" t="str">
-        <f>VLOOKUP(F325,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F325,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H325" s="14">
@@ -63026,7 +63026,7 @@
         <v>39</v>
       </c>
       <c r="G326" s="26" t="str">
-        <f>VLOOKUP(F326,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F326,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H326" s="14">
@@ -63113,7 +63113,7 @@
         <v>39</v>
       </c>
       <c r="G327" s="26" t="str">
-        <f>VLOOKUP(F327,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F327,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H327" s="14">
@@ -63204,7 +63204,7 @@
         <v>47</v>
       </c>
       <c r="G328" s="26" t="str">
-        <f>VLOOKUP(F328,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F328,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H328" s="14">
@@ -63297,7 +63297,7 @@
         <v>46</v>
       </c>
       <c r="G329" s="26" t="str">
-        <f>VLOOKUP(F329,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F329,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H329" s="14">
@@ -63383,9 +63383,9 @@
       <c r="F330" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G330" s="26" t="e">
-        <f>VLOOKUP(F330,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G330" s="26" t="str">
+        <f>VLOOKUP(F330,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H330" s="14">
         <v>8559487.8000000007</v>
@@ -63470,9 +63470,9 @@
       <c r="F331" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G331" s="26" t="e">
-        <f>VLOOKUP(F331,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G331" s="26" t="str">
+        <f>VLOOKUP(F331,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H331" s="14">
         <v>8559482.7699999996</v>
@@ -63558,7 +63558,7 @@
         <v>65</v>
       </c>
       <c r="G332" s="26" t="str">
-        <f>VLOOKUP(F332,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F332,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H332" s="14">
@@ -63649,8 +63649,8 @@
         <v>57</v>
       </c>
       <c r="G333" s="26" t="str">
-        <f>VLOOKUP(F333,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F333,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H333" s="14">
         <v>8558473.9900000002</v>
@@ -63736,7 +63736,7 @@
         <v>39</v>
       </c>
       <c r="G334" s="26" t="str">
-        <f>VLOOKUP(F334,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F334,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H334" s="14">
@@ -63823,7 +63823,7 @@
         <v>42</v>
       </c>
       <c r="G335" s="26" t="str">
-        <f>VLOOKUP(F335,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F335,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H335" s="14">
@@ -63910,7 +63910,7 @@
         <v>46</v>
       </c>
       <c r="G336" s="26" t="str">
-        <f>VLOOKUP(F336,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F336,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H336" s="14">
@@ -63997,7 +63997,7 @@
         <v>56</v>
       </c>
       <c r="G337" s="26" t="str">
-        <f>VLOOKUP(F337,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F337,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H337" s="14">
@@ -64088,7 +64088,7 @@
         <v>56</v>
       </c>
       <c r="G338" s="26" t="str">
-        <f>VLOOKUP(F338,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F338,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H338" s="14">
@@ -64179,7 +64179,7 @@
         <v>39</v>
       </c>
       <c r="G339" s="26" t="str">
-        <f>VLOOKUP(F339,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F339,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H339" s="14">
@@ -64271,9 +64271,9 @@
       <c r="F340" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G340" s="26" t="e">
-        <f>VLOOKUP(F340,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G340" s="26" t="str">
+        <f>VLOOKUP(F340,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H340" s="14">
         <v>8555634.6699999999</v>
@@ -64359,7 +64359,7 @@
         <v>65</v>
       </c>
       <c r="G341" s="26" t="str">
-        <f>VLOOKUP(F341,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F341,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H341" s="14">
@@ -64438,7 +64438,7 @@
         <v>39</v>
       </c>
       <c r="G342" s="26" t="str">
-        <f>VLOOKUP(F342,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F342,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H342" s="14">
@@ -64525,7 +64525,7 @@
         <v>65</v>
       </c>
       <c r="G343" s="26" t="str">
-        <f>VLOOKUP(F343,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F343,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H343" s="14">
@@ -64608,7 +64608,7 @@
         <v>51</v>
       </c>
       <c r="G344" s="26" t="str">
-        <f>VLOOKUP(F344,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F344,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H344" s="14">
@@ -64695,8 +64695,8 @@
         <v>57</v>
       </c>
       <c r="G345" s="26" t="str">
-        <f>VLOOKUP(F345,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F345,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H345" s="14">
         <v>8554715.6600000001</v>
@@ -64786,8 +64786,8 @@
         <v>57</v>
       </c>
       <c r="G346" s="26" t="str">
-        <f>VLOOKUP(F346,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F346,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H346" s="14">
         <v>8552713.1600000001</v>
@@ -64877,7 +64877,7 @@
         <v>42</v>
       </c>
       <c r="G347" s="26" t="str">
-        <f>VLOOKUP(F347,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F347,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H347" s="14">
@@ -64960,7 +64960,7 @@
         <v>46</v>
       </c>
       <c r="G348" s="26" t="str">
-        <f>VLOOKUP(F348,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F348,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H348" s="14">
@@ -65047,7 +65047,7 @@
         <v>46</v>
       </c>
       <c r="G349" s="26" t="str">
-        <f>VLOOKUP(F349,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F349,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H349" s="14">
@@ -65134,7 +65134,7 @@
         <v>42</v>
       </c>
       <c r="G350" s="26" t="str">
-        <f>VLOOKUP(F350,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F350,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H350" s="14">
@@ -65212,9 +65212,9 @@
       <c r="F351" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G351" s="26" t="e">
-        <f>VLOOKUP(F351,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G351" s="26" t="str">
+        <f>VLOOKUP(F351,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H351" s="14">
         <v>8550863.2100000009</v>
@@ -65306,7 +65306,7 @@
         <v>46</v>
       </c>
       <c r="G352" s="26" t="str">
-        <f>VLOOKUP(F352,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F352,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H352" s="14">
@@ -65388,9 +65388,9 @@
       <c r="F353" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G353" s="26" t="e">
-        <f>VLOOKUP(F353,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G353" s="26" t="str">
+        <f>VLOOKUP(F353,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H353" s="14">
         <v>8550336.8699999992</v>
@@ -65475,9 +65475,9 @@
       <c r="F354" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G354" s="26" t="e">
-        <f>VLOOKUP(F354,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G354" s="26" t="str">
+        <f>VLOOKUP(F354,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H354" s="14">
         <v>8550120.6999999993</v>
@@ -65559,7 +65559,7 @@
         <v>39</v>
       </c>
       <c r="G355" s="26" t="str">
-        <f>VLOOKUP(F355,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F355,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H355" s="14">
@@ -65646,7 +65646,7 @@
         <v>39</v>
       </c>
       <c r="G356" s="26" t="str">
-        <f>VLOOKUP(F356,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F356,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H356" s="14">
@@ -65733,7 +65733,7 @@
         <v>39</v>
       </c>
       <c r="G357" s="26" t="str">
-        <f>VLOOKUP(F357,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F357,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H357" s="14">
@@ -65826,7 +65826,7 @@
         <v>47</v>
       </c>
       <c r="G358" s="26" t="str">
-        <f>VLOOKUP(F358,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F358,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H358" s="14">
@@ -65905,7 +65905,7 @@
         <v>46</v>
       </c>
       <c r="G359" s="26" t="str">
-        <f>VLOOKUP(F359,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F359,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H359" s="14">
@@ -65983,9 +65983,9 @@
       <c r="F360" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G360" s="26" t="e">
-        <f>VLOOKUP(F360,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G360" s="26" t="str">
+        <f>VLOOKUP(F360,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H360" s="14">
         <v>8548650.1600000001</v>
@@ -66071,7 +66071,7 @@
         <v>46</v>
       </c>
       <c r="G361" s="26" t="str">
-        <f>VLOOKUP(F361,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F361,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H361" s="14">
@@ -66158,7 +66158,7 @@
         <v>39</v>
       </c>
       <c r="G362" s="26" t="str">
-        <f>VLOOKUP(F362,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F362,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H362" s="14">
@@ -66245,7 +66245,7 @@
         <v>42</v>
       </c>
       <c r="G363" s="26" t="str">
-        <f>VLOOKUP(F363,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F363,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H363" s="14">
@@ -66332,7 +66332,7 @@
         <v>39</v>
       </c>
       <c r="G364" s="26" t="str">
-        <f>VLOOKUP(F364,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F364,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H364" s="14">
@@ -66419,7 +66419,7 @@
         <v>39</v>
       </c>
       <c r="G365" s="26" t="str">
-        <f>VLOOKUP(F365,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F365,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H365" s="14">
@@ -66510,7 +66510,7 @@
         <v>46</v>
       </c>
       <c r="G366" s="26" t="str">
-        <f>VLOOKUP(F366,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F366,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H366" s="14">
@@ -66596,9 +66596,9 @@
       <c r="F367" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G367" s="26" t="e">
-        <f>VLOOKUP(F367,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G367" s="26" t="str">
+        <f>VLOOKUP(F367,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H367" s="14">
         <v>8545527.1999999993</v>
@@ -66680,7 +66680,7 @@
         <v>39</v>
       </c>
       <c r="G368" s="26" t="str">
-        <f>VLOOKUP(F368,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F368,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H368" s="14">
@@ -66767,7 +66767,7 @@
         <v>46</v>
       </c>
       <c r="G369" s="26" t="str">
-        <f>VLOOKUP(F369,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F369,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H369" s="14">
@@ -66846,7 +66846,7 @@
         <v>42</v>
       </c>
       <c r="G370" s="26" t="str">
-        <f>VLOOKUP(F370,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F370,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H370" s="14">
@@ -66933,8 +66933,8 @@
         <v>57</v>
       </c>
       <c r="G371" s="26" t="str">
-        <f>VLOOKUP(F371,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F371,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H371" s="14">
         <v>8541466.0099999998</v>
@@ -67020,7 +67020,7 @@
         <v>39</v>
       </c>
       <c r="G372" s="26" t="str">
-        <f>VLOOKUP(F372,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F372,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H372" s="14">
@@ -67107,7 +67107,7 @@
         <v>39</v>
       </c>
       <c r="G373" s="26" t="str">
-        <f>VLOOKUP(F373,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F373,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H373" s="14">
@@ -67186,7 +67186,7 @@
         <v>46</v>
       </c>
       <c r="G374" s="26" t="str">
-        <f>VLOOKUP(F374,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F374,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H374" s="14">
@@ -67265,7 +67265,7 @@
         <v>56</v>
       </c>
       <c r="G375" s="26" t="str">
-        <f>VLOOKUP(F375,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F375,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>28 Warmian-Masurian Province</v>
       </c>
       <c r="H375" s="14">
@@ -67352,7 +67352,7 @@
         <v>39</v>
       </c>
       <c r="G376" s="26" t="str">
-        <f>VLOOKUP(F376,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F376,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H376" s="14">
@@ -67431,7 +67431,7 @@
         <v>46</v>
       </c>
       <c r="G377" s="26" t="str">
-        <f>VLOOKUP(F377,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F377,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>22 Pomeranian Province</v>
       </c>
       <c r="H377" s="14">
@@ -67522,7 +67522,7 @@
         <v>39</v>
       </c>
       <c r="G378" s="26" t="str">
-        <f>VLOOKUP(F378,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F378,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H378" s="14">
@@ -67609,7 +67609,7 @@
         <v>47</v>
       </c>
       <c r="G379" s="26" t="str">
-        <f>VLOOKUP(F379,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F379,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H379" s="14">
@@ -67696,7 +67696,7 @@
         <v>47</v>
       </c>
       <c r="G380" s="26" t="str">
-        <f>VLOOKUP(F380,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F380,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H380" s="14">
@@ -67787,7 +67787,7 @@
         <v>47</v>
       </c>
       <c r="G381" s="26" t="str">
-        <f>VLOOKUP(F381,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F381,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H381" s="14">
@@ -67866,7 +67866,7 @@
         <v>47</v>
       </c>
       <c r="G382" s="26" t="str">
-        <f>VLOOKUP(F382,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F382,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H382" s="14">
@@ -67955,7 +67955,7 @@
         <v>39</v>
       </c>
       <c r="G383" s="26" t="str">
-        <f>VLOOKUP(F383,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F383,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H383" s="14">
@@ -68034,7 +68034,7 @@
         <v>47</v>
       </c>
       <c r="G384" s="26" t="str">
-        <f>VLOOKUP(F384,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F384,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H384" s="14">
@@ -68121,7 +68121,7 @@
         <v>47</v>
       </c>
       <c r="G385" s="26" t="str">
-        <f>VLOOKUP(F385,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F385,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H385" s="14">
@@ -68208,7 +68208,7 @@
         <v>39</v>
       </c>
       <c r="G386" s="26" t="str">
-        <f>VLOOKUP(F386,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F386,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H386" s="14">
@@ -68299,7 +68299,7 @@
         <v>39</v>
       </c>
       <c r="G387" s="26" t="str">
-        <f>VLOOKUP(F387,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F387,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H387" s="14">
@@ -68386,7 +68386,7 @@
         <v>39</v>
       </c>
       <c r="G388" s="26" t="str">
-        <f>VLOOKUP(F388,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F388,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H388" s="14">
@@ -68473,7 +68473,7 @@
         <v>47</v>
       </c>
       <c r="G389" s="26" t="str">
-        <f>VLOOKUP(F389,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F389,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H389" s="14">
@@ -68564,7 +68564,7 @@
         <v>47</v>
       </c>
       <c r="G390" s="26" t="str">
-        <f>VLOOKUP(F390,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F390,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H390" s="14">
@@ -68643,7 +68643,7 @@
         <v>65</v>
       </c>
       <c r="G391" s="26" t="str">
-        <f>VLOOKUP(F391,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F391,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H391" s="14">
@@ -68730,7 +68730,7 @@
         <v>47</v>
       </c>
       <c r="G392" s="26" t="str">
-        <f>VLOOKUP(F392,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F392,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H392" s="14">
@@ -68809,7 +68809,7 @@
         <v>39</v>
       </c>
       <c r="G393" s="26" t="str">
-        <f>VLOOKUP(F393,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F393,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H393" s="14">
@@ -68888,7 +68888,7 @@
         <v>47</v>
       </c>
       <c r="G394" s="26" t="str">
-        <f>VLOOKUP(F394,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F394,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H394" s="14">
@@ -68975,7 +68975,7 @@
         <v>47</v>
       </c>
       <c r="G395" s="26" t="str">
-        <f>VLOOKUP(F395,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F395,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H395" s="14">
@@ -69066,7 +69066,7 @@
         <v>42</v>
       </c>
       <c r="G396" s="26" t="str">
-        <f>VLOOKUP(F396,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F396,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H396" s="14">
@@ -69157,7 +69157,7 @@
         <v>47</v>
       </c>
       <c r="G397" s="26" t="str">
-        <f>VLOOKUP(F397,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F397,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H397" s="14">
@@ -69248,7 +69248,7 @@
         <v>47</v>
       </c>
       <c r="G398" s="26" t="str">
-        <f>VLOOKUP(F398,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F398,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H398" s="14">
@@ -69327,7 +69327,7 @@
         <v>39</v>
       </c>
       <c r="G399" s="26" t="str">
-        <f>VLOOKUP(F399,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F399,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H399" s="14">
@@ -69406,7 +69406,7 @@
         <v>51</v>
       </c>
       <c r="G400" s="26" t="str">
-        <f>VLOOKUP(F400,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F400,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H400" s="14">
@@ -69485,8 +69485,8 @@
         <v>57</v>
       </c>
       <c r="G401" s="26" t="str">
-        <f>VLOOKUP(F401,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F401,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H401" s="14">
         <v>8525988.9299999997</v>
@@ -69571,9 +69571,9 @@
       <c r="F402" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G402" s="26" t="e">
-        <f>VLOOKUP(F402,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G402" s="26" t="str">
+        <f>VLOOKUP(F402,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H402" s="14">
         <v>8525877.8699999992</v>
@@ -69663,7 +69663,7 @@
         <v>39</v>
       </c>
       <c r="G403" s="26" t="str">
-        <f>VLOOKUP(F403,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F403,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H403" s="14">
@@ -69742,7 +69742,7 @@
         <v>42</v>
       </c>
       <c r="G404" s="26" t="str">
-        <f>VLOOKUP(F404,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F404,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H404" s="14">
@@ -69825,7 +69825,7 @@
         <v>51</v>
       </c>
       <c r="G405" s="26" t="str">
-        <f>VLOOKUP(F405,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F405,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H405" s="14">
@@ -69908,7 +69908,7 @@
         <v>47</v>
       </c>
       <c r="G406" s="26" t="str">
-        <f>VLOOKUP(F406,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F406,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H406" s="14">
@@ -69995,7 +69995,7 @@
         <v>47</v>
       </c>
       <c r="G407" s="26" t="str">
-        <f>VLOOKUP(F407,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F407,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H407" s="14">
@@ -70074,7 +70074,7 @@
         <v>51</v>
       </c>
       <c r="G408" s="26" t="str">
-        <f>VLOOKUP(F408,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F408,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H408" s="14">
@@ -70165,7 +70165,7 @@
         <v>39</v>
       </c>
       <c r="G409" s="26" t="str">
-        <f>VLOOKUP(F409,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F409,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H409" s="14">
@@ -70244,8 +70244,8 @@
         <v>63</v>
       </c>
       <c r="G410" s="26" t="str">
-        <f>VLOOKUP(F410,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>26 Świętokrzyskie Province</v>
+        <f>VLOOKUP(F410,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>26 Swietokrzyskie Province</v>
       </c>
       <c r="H410" s="14">
         <v>8520895.9399999995</v>
@@ -70323,7 +70323,7 @@
         <v>65</v>
       </c>
       <c r="G411" s="26" t="str">
-        <f>VLOOKUP(F411,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F411,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H411" s="14">
@@ -70410,7 +70410,7 @@
         <v>51</v>
       </c>
       <c r="G412" s="26" t="str">
-        <f>VLOOKUP(F412,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F412,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>02 Lower Silesia Province</v>
       </c>
       <c r="H412" s="14">
@@ -70501,7 +70501,7 @@
         <v>39</v>
       </c>
       <c r="G413" s="26" t="str">
-        <f>VLOOKUP(F413,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F413,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H413" s="14">
@@ -70592,7 +70592,7 @@
         <v>39</v>
       </c>
       <c r="G414" s="26" t="str">
-        <f>VLOOKUP(F414,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F414,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H414" s="14">
@@ -70679,7 +70679,7 @@
         <v>39</v>
       </c>
       <c r="G415" s="26" t="str">
-        <f>VLOOKUP(F415,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F415,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H415" s="14">
@@ -70766,7 +70766,7 @@
         <v>47</v>
       </c>
       <c r="G416" s="26" t="str">
-        <f>VLOOKUP(F416,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F416,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H416" s="14">
@@ -70845,7 +70845,7 @@
         <v>47</v>
       </c>
       <c r="G417" s="26" t="str">
-        <f>VLOOKUP(F417,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F417,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H417" s="14">
@@ -70932,7 +70932,7 @@
         <v>47</v>
       </c>
       <c r="G418" s="26" t="str">
-        <f>VLOOKUP(F418,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F418,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H418" s="14">
@@ -71015,7 +71015,7 @@
         <v>65</v>
       </c>
       <c r="G419" s="26" t="str">
-        <f>VLOOKUP(F419,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F419,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H419" s="14">
@@ -71094,7 +71094,7 @@
         <v>47</v>
       </c>
       <c r="G420" s="26" t="str">
-        <f>VLOOKUP(F420,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F420,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H420" s="14">
@@ -71181,7 +71181,7 @@
         <v>39</v>
       </c>
       <c r="G421" s="26" t="str">
-        <f>VLOOKUP(F421,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F421,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H421" s="14">
@@ -71274,7 +71274,7 @@
         <v>47</v>
       </c>
       <c r="G422" s="26" t="str">
-        <f>VLOOKUP(F422,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F422,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H422" s="14">
@@ -71356,9 +71356,9 @@
       <c r="F423" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G423" s="26" t="e">
-        <f>VLOOKUP(F423,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G423" s="26" t="str">
+        <f>VLOOKUP(F423,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H423" s="14">
         <v>8512590.8200000003</v>
@@ -71444,7 +71444,7 @@
         <v>47</v>
       </c>
       <c r="G424" s="26" t="str">
-        <f>VLOOKUP(F424,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F424,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H424" s="14">
@@ -71527,7 +71527,7 @@
         <v>47</v>
       </c>
       <c r="G425" s="26" t="str">
-        <f>VLOOKUP(F425,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F425,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H425" s="14">
@@ -71614,7 +71614,7 @@
         <v>65</v>
       </c>
       <c r="G426" s="26" t="str">
-        <f>VLOOKUP(F426,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F426,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H426" s="14">
@@ -71701,7 +71701,7 @@
         <v>39</v>
       </c>
       <c r="G427" s="26" t="str">
-        <f>VLOOKUP(F427,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F427,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H427" s="14">
@@ -71780,7 +71780,7 @@
         <v>39</v>
       </c>
       <c r="G428" s="26" t="str">
-        <f>VLOOKUP(F428,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F428,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H428" s="14">
@@ -71867,7 +71867,7 @@
         <v>39</v>
       </c>
       <c r="G429" s="26" t="str">
-        <f>VLOOKUP(F429,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F429,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H429" s="14">
@@ -71954,7 +71954,7 @@
         <v>47</v>
       </c>
       <c r="G430" s="26" t="str">
-        <f>VLOOKUP(F430,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F430,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H430" s="14">
@@ -72033,7 +72033,7 @@
         <v>39</v>
       </c>
       <c r="G431" s="26" t="str">
-        <f>VLOOKUP(F431,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F431,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H431" s="14">
@@ -72119,9 +72119,9 @@
       <c r="F432" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G432" s="26" t="e">
-        <f>VLOOKUP(F432,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="G432" s="26" t="str">
+        <f>VLOOKUP(F432,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>08 Lubuskie</v>
       </c>
       <c r="H432" s="14">
         <v>8509098.9600000009</v>
@@ -72203,7 +72203,7 @@
         <v>39</v>
       </c>
       <c r="G433" s="26" t="str">
-        <f>VLOOKUP(F433,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F433,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H433" s="14">
@@ -72290,7 +72290,7 @@
         <v>47</v>
       </c>
       <c r="G434" s="26" t="str">
-        <f>VLOOKUP(F434,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F434,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H434" s="14">
@@ -72369,7 +72369,7 @@
         <v>42</v>
       </c>
       <c r="G435" s="26" t="str">
-        <f>VLOOKUP(F435,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F435,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H435" s="14">
@@ -72456,7 +72456,7 @@
         <v>65</v>
       </c>
       <c r="G436" s="26" t="str">
-        <f>VLOOKUP(F436,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F436,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>32 West Pomeranian Province</v>
       </c>
       <c r="H436" s="14">
@@ -72543,7 +72543,7 @@
         <v>39</v>
       </c>
       <c r="G437" s="26" t="str">
-        <f>VLOOKUP(F437,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F437,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H437" s="14">
@@ -72622,7 +72622,7 @@
         <v>47</v>
       </c>
       <c r="G438" s="26" t="str">
-        <f>VLOOKUP(F438,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F438,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H438" s="14">
@@ -72701,7 +72701,7 @@
         <v>42</v>
       </c>
       <c r="G439" s="26" t="str">
-        <f>VLOOKUP(F439,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F439,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H439" s="14">
@@ -72800,7 +72800,7 @@
         <v>47</v>
       </c>
       <c r="G440" s="26" t="str">
-        <f>VLOOKUP(F440,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F440,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H440" s="14">
@@ -72887,7 +72887,7 @@
         <v>39</v>
       </c>
       <c r="G441" s="26" t="str">
-        <f>VLOOKUP(F441,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F441,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H441" s="14">
@@ -72978,7 +72978,7 @@
         <v>39</v>
       </c>
       <c r="G442" s="26" t="str">
-        <f>VLOOKUP(F442,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F442,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H442" s="14">
@@ -73065,8 +73065,8 @@
         <v>63</v>
       </c>
       <c r="G443" s="26" t="str">
-        <f>VLOOKUP(F443,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>26 Świętokrzyskie Province</v>
+        <f>VLOOKUP(F443,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>26 Swietokrzyskie Province</v>
       </c>
       <c r="H443" s="14">
         <v>8505591.4600000009</v>
@@ -73152,8 +73152,8 @@
         <v>57</v>
       </c>
       <c r="G444" s="26" t="str">
-        <f>VLOOKUP(F444,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F444,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H444" s="14">
         <v>8504970.2400000002</v>
@@ -73249,7 +73249,7 @@
         <v>39</v>
       </c>
       <c r="G445" s="26" t="str">
-        <f>VLOOKUP(F445,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F445,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H445" s="14">
@@ -73340,7 +73340,7 @@
         <v>47</v>
       </c>
       <c r="G446" s="26" t="str">
-        <f>VLOOKUP(F446,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F446,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H446" s="14">
@@ -73427,7 +73427,7 @@
         <v>42</v>
       </c>
       <c r="G447" s="26" t="str">
-        <f>VLOOKUP(F447,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F447,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H447" s="14">
@@ -73516,7 +73516,7 @@
         <v>47</v>
       </c>
       <c r="G448" s="26" t="str">
-        <f>VLOOKUP(F448,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F448,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H448" s="14">
@@ -73599,7 +73599,7 @@
         <v>47</v>
       </c>
       <c r="G449" s="26" t="str">
-        <f>VLOOKUP(F449,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F449,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H449" s="14">
@@ -73686,7 +73686,7 @@
         <v>47</v>
       </c>
       <c r="G450" s="26" t="str">
-        <f>VLOOKUP(F450,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F450,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H450" s="14">
@@ -73765,7 +73765,7 @@
         <v>42</v>
       </c>
       <c r="G451" s="26" t="str">
-        <f>VLOOKUP(F451,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F451,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>30 Greater Poland Province</v>
       </c>
       <c r="H451" s="16">
@@ -73852,8 +73852,8 @@
         <v>57</v>
       </c>
       <c r="G452" s="26" t="str">
-        <f>VLOOKUP(F452,col_4!$C$2:$D$16,2,FALSE)</f>
-        <v>10 Łódź Province</v>
+        <f>VLOOKUP(F452,col_4!$C$2:$D$17,2,FALSE)</f>
+        <v>10 Lodz</v>
       </c>
       <c r="H452" s="16">
         <v>3145892.41</v>
@@ -73939,7 +73939,7 @@
         <v>39</v>
       </c>
       <c r="G453" s="26" t="str">
-        <f>VLOOKUP(F453,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F453,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>14 Mazovia Province</v>
       </c>
       <c r="H453" s="16">
@@ -74026,7 +74026,7 @@
         <v>47</v>
       </c>
       <c r="G454" s="26" t="str">
-        <f>VLOOKUP(F454,col_4!$C$2:$D$16,2,FALSE)</f>
+        <f>VLOOKUP(F454,col_4!$C$2:$D$17,2,FALSE)</f>
         <v>24 Silesia Province</v>
       </c>
       <c r="H454" s="16">
@@ -74128,7 +74128,7 @@
       <c r="B2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>143</v>
       </c>
     </row>
@@ -74469,16 +74469,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF2E24D-F372-4004-AD54-45C6CE6A0CC2}">
-  <dimension ref="C1:D16"/>
+  <dimension ref="C1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.5546875" customWidth="1"/>
     <col min="4" max="4" width="43.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.25">
@@ -74511,99 +74512,107 @@
       </c>
     </row>
     <row r="5" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C5" s="26" t="s">
-        <v>57</v>
+      <c r="C5" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>185</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C6" s="26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C7" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C8" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C12" s="26" t="s">
-        <v>47</v>
-      </c>
       <c r="D12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="C13" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C14" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="D13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
+      <c r="D14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C15" s="26" t="s">
-        <v>42</v>
       </c>
       <c r="D15" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="16" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D16" t="s">
-        <v>193</v>
+      <c r="D17" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added deduction exemptions, summary of exemptions
</commit_message>
<xml_diff>
--- a/Poland CIT Sample.xlsx
+++ b/Poland CIT Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb544155\OneDrive - WBG\Documents\GitHub\Microsimulation_Poland\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{C0971418-5566-47FF-A835-0BC158507F59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{1F224A77-88A5-4538-8273-55BE26852AD6}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{C0971418-5566-47FF-A835-0BC158507F59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{89BBD5ED-B669-4E4A-948E-651376E5C526}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,9 +406,6 @@
   </si>
   <si>
     <t>     loss from previous years</t>
-  </si>
-  <si>
-    <t>        income deductions (Article 18 (1) (1))</t>
   </si>
   <si>
     <t>        income deductions (Article 18 (1) (7))</t>
@@ -885,6 +882,9 @@
   <si>
     <t xml:space="preserve">subsidies, subsidies, surcharges and other irrelevant wit-free of tax (Article 17 (1) point 21) </t>
   </si>
+  <si>
+    <t>income deductions (Article 18 (1) (1))</t>
+  </si>
 </sst>
 </file>
 
@@ -1008,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1087,6 +1087,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,7 +1419,7 @@
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
     </row>
-    <row r="2" spans="1:43" s="4" customFormat="1" ht="137.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" s="4" customFormat="1" ht="125" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>85</v>
       </c>
@@ -35089,8 +35090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCEBCF2-7BCD-464C-9CC3-58FC2DD939B9}">
   <dimension ref="A1:AV455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL1" sqref="AL1:AQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -35135,172 +35136,172 @@
   <sheetData>
     <row r="1" spans="1:48" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
         <v>196</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
         <v>197</v>
       </c>
-      <c r="C1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>198</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>199</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>200</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>201</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>202</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>203</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>204</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>205</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>206</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>207</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>208</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>209</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>210</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>211</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>212</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>213</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>214</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>215</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>216</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>217</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>218</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>219</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>220</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>221</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>222</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>223</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>224</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>225</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>226</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>227</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>228</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>229</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>230</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>237</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>238</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>239</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>240</v>
       </c>
-      <c r="AU1" t="s">
-        <v>241</v>
-      </c>
       <c r="AV1" s="1"/>
     </row>
-    <row r="2" spans="1:48" s="28" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" s="28" customFormat="1" ht="50" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>103</v>
       </c>
       <c r="D2" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>162</v>
-      </c>
       <c r="H2" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>104</v>
@@ -35324,7 +35325,7 @@
         <v>110</v>
       </c>
       <c r="P2" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q2" s="31" t="s">
         <v>111</v>
@@ -35342,52 +35343,52 @@
         <v>115</v>
       </c>
       <c r="V2" s="31" t="s">
+        <v>246</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="X2" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="Y2" s="31" t="s">
         <v>247</v>
       </c>
-      <c r="W2" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="X2" s="32" t="s">
+      <c r="Z2" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="Y2" s="31" t="s">
+      <c r="AA2" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="Z2" s="31" t="s">
-        <v>276</v>
-      </c>
-      <c r="AA2" s="31" t="s">
-        <v>249</v>
-      </c>
       <c r="AB2" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AC2" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="AD2" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="AD2" s="31" t="s">
-        <v>255</v>
-      </c>
       <c r="AE2" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="AF2" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="AF2" s="31" t="s">
-        <v>259</v>
-      </c>
       <c r="AG2" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="AH2" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="AH2" s="31" t="s">
-        <v>263</v>
-      </c>
       <c r="AI2" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AJ2" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="AK2" s="31" t="s">
         <v>268</v>
-      </c>
-      <c r="AK2" s="31" t="s">
-        <v>269</v>
       </c>
       <c r="AL2" s="31" t="s">
         <v>116</v>
@@ -35396,28 +35397,28 @@
         <v>117</v>
       </c>
       <c r="AN2" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="AO2" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="AO2" s="31" t="s">
+      <c r="AP2" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="AP2" s="31" t="s">
+      <c r="AQ2" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="AQ2" s="31" t="s">
+      <c r="AR2" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="AR2" s="31" t="s">
+      <c r="AS2" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="AS2" s="31" t="s">
+      <c r="AT2" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="AT2" s="31" t="s">
+      <c r="AU2" s="31" t="s">
         <v>124</v>
-      </c>
-      <c r="AU2" s="31" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:48" s="4" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
@@ -35477,52 +35478,52 @@
         <v>13</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="W3" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="X3" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="X3" s="13" t="s">
+      <c r="Y3" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="Y3" s="13" t="s">
+      <c r="Z3" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="Z3" s="13" t="s">
-        <v>274</v>
-      </c>
       <c r="AA3" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AB3" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AC3" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="AC3" s="13" t="s">
-        <v>253</v>
-      </c>
       <c r="AD3" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="AE3" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="AE3" s="13" t="s">
-        <v>257</v>
-      </c>
       <c r="AF3" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="AG3" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="AG3" s="13" t="s">
-        <v>261</v>
-      </c>
       <c r="AH3" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AI3" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="AJ3" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="AJ3" s="13" t="s">
-        <v>267</v>
-      </c>
       <c r="AK3" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="AL3" s="12" t="s">
         <v>29</v>
@@ -35715,7 +35716,7 @@
         <v>99</v>
       </c>
       <c r="R5" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S5" s="22"/>
       <c r="T5" s="23" t="s">
@@ -76326,7 +76327,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76337,7 +76338,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76348,7 +76349,7 @@
         <v>84</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76359,7 +76360,7 @@
         <v>82</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76370,7 +76371,7 @@
         <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76381,7 +76382,7 @@
         <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76392,7 +76393,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76403,7 +76404,7 @@
         <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76414,7 +76415,7 @@
         <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76425,7 +76426,7 @@
         <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76436,7 +76437,7 @@
         <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76447,7 +76448,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.25">
@@ -76458,7 +76459,7 @@
         <v>79</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="27" customFormat="1" ht="14" x14ac:dyDescent="0.25">
@@ -76469,7 +76470,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -76510,10 +76511,10 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76521,10 +76522,10 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76532,10 +76533,10 @@
         <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76543,10 +76544,10 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76554,10 +76555,10 @@
         <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76565,10 +76566,10 @@
         <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76576,10 +76577,10 @@
         <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76587,10 +76588,10 @@
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76598,10 +76599,10 @@
         <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76609,10 +76610,10 @@
         <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76620,10 +76621,10 @@
         <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76631,10 +76632,10 @@
         <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76642,10 +76643,10 @@
         <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76653,10 +76654,10 @@
         <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76664,10 +76665,10 @@
         <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76675,10 +76676,10 @@
         <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76686,10 +76687,10 @@
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76697,10 +76698,10 @@
         <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="3:5" ht="14" x14ac:dyDescent="0.25">
@@ -76708,10 +76709,10 @@
         <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -76747,7 +76748,7 @@
         <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76755,7 +76756,7 @@
         <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76763,7 +76764,7 @@
         <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76779,7 +76780,7 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76787,7 +76788,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76795,7 +76796,7 @@
         <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76803,7 +76804,7 @@
         <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76811,7 +76812,7 @@
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76819,7 +76820,7 @@
         <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76827,7 +76828,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76835,7 +76836,7 @@
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76843,7 +76844,7 @@
         <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76851,7 +76852,7 @@
         <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76859,7 +76860,7 @@
         <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="14" x14ac:dyDescent="0.25">
@@ -76867,7 +76868,7 @@
         <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>